<commit_message>
Added Publons login tests scripts using facebook and Gmail.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -127,13 +127,31 @@
   </si>
   <si>
     <t>PUBLONS001</t>
+  </si>
+  <si>
+    <t>OPQA-5885||OPQA-5888</t>
+  </si>
+  <si>
+    <t>OPQA-5884||OPQA-5887</t>
+  </si>
+  <si>
+    <t>User Sign In  Publon's using valid facebook username and password from login page then it should redirected to Publon's Home page.</t>
+  </si>
+  <si>
+    <t>User Sign In Publon's using valid gmail username and password from login page then it should redirected to Publon's Home page.</t>
+  </si>
+  <si>
+    <t>PUBLONS020</t>
+  </si>
+  <si>
+    <t>PUBLONS021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +173,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -219,6 +250,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +631,232 @@
         <v>5</v>
       </c>
       <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Publons test scripts.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="46">
   <si>
     <t>TCID</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>PUBLONS021</t>
+  </si>
+  <si>
+    <t>PUBLONS022</t>
+  </si>
+  <si>
+    <t>OPQA-5890</t>
+  </si>
+  <si>
+    <t>Verify Error message when user  exist in platform in suspend state and trying to login.</t>
   </si>
 </sst>
 </file>
@@ -587,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,10 +791,18 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created new scripts in publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="WAT09" sheetId="2" r:id="rId2"/>
-    <sheet name="WAT13" sheetId="4" r:id="rId3"/>
+    <sheet name="PUBLONS005" sheetId="5" r:id="rId2"/>
+    <sheet name="WAT09" sheetId="2" r:id="rId3"/>
+    <sheet name="WAT13" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -172,13 +173,79 @@
   </si>
   <si>
     <t>Verify Error message when user  exist in platform in Evicted state and trying to login.</t>
+  </si>
+  <si>
+    <t>PUBLONS002</t>
+  </si>
+  <si>
+    <t>PUBLONS003</t>
+  </si>
+  <si>
+    <t>OPQA-5765</t>
+  </si>
+  <si>
+    <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter an email address" whenever not enter any text in email field</t>
+  </si>
+  <si>
+    <t>OPQA-5766</t>
+  </si>
+  <si>
+    <t>PUBLONS004</t>
+  </si>
+  <si>
+    <t>OPQA-5767</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter a valid email address" whenever enter wrong format in email field</t>
+  </si>
+  <si>
+    <t>CHARACTER LENGTH</t>
+  </si>
+  <si>
+    <t>SUFFIX</t>
+  </si>
+  <si>
+    <t>ERROR TEXT</t>
+  </si>
+  <si>
+    <t>VALIDITY</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>@abc.com</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Please enter no more than 255 characters.</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PUBLONS005</t>
+  </si>
+  <si>
+    <t>Verify that error message "Email address is too long." whenever enter more than 255 characters in email field&amp;&amp;Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
+  </si>
+  <si>
+    <t>OPQA-5768&amp;&amp;OPQA-5765</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +273,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -258,10 +332,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -280,8 +358,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -614,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,31 +741,63 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,6 +1029,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>246</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>247</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>248</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -1251,7 +1466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Developed new scripts in publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="PUBLONS005" sheetId="5" r:id="rId2"/>
-    <sheet name="WAT09" sheetId="2" r:id="rId3"/>
-    <sheet name="WAT13" sheetId="4" r:id="rId4"/>
+    <sheet name="PUBLONS009" sheetId="6" r:id="rId2"/>
+    <sheet name="PUBLONS005" sheetId="5" r:id="rId3"/>
+    <sheet name="WAT09" sheetId="2" r:id="rId4"/>
+    <sheet name="WAT13" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="80">
   <si>
     <t>TCID</t>
   </si>
@@ -239,6 +240,24 @@
   </si>
   <si>
     <t>OPQA-5768&amp;&amp;OPQA-5765</t>
+  </si>
+  <si>
+    <t>OPQA-5781</t>
+  </si>
+  <si>
+    <t>PUBLONS008</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter your last name." whenever not enter any text in email field</t>
+  </si>
+  <si>
+    <t>PUBLONS009</t>
+  </si>
+  <si>
+    <t>OPQA-5782&amp;&amp;OPQA-5783</t>
+  </si>
+  <si>
+    <t>Verify that last name should be maximum of 50 characters long and these fields should not be empty.&amp;&amp;Verify that error message Last name is too long." whenever enter more than 50 characters</t>
   </si>
 </sst>
 </file>
@@ -696,7 +715,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,17 +820,33 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,6 +1064,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>49</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>50</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>51</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1130,7 +1236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -1466,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added new scripts in Publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="95">
   <si>
     <t>TCID</t>
   </si>
@@ -286,6 +286,24 @@
   </si>
   <si>
     <t>Verify that "Your email address is already registered. Please sign in." error message whenever try to create publons user using existing account.&amp;&amp;Verify that email address prepopulated in sign in page whenever try to register user using existing user</t>
+  </si>
+  <si>
+    <t>PUBLONS013</t>
+  </si>
+  <si>
+    <t>OPQA-5771||OPQA-5772||OPQA-5773||OPQA-5774||OPQA-5775||OPQA-5776||OPQA-5777||OPQA-6000</t>
+  </si>
+  <si>
+    <t>Verify Password must have at least one special character from !@#$%^*()~`{}[] in Registration  page||Verify Password must contain at least one number is ALWAYS enforced in Registration  page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in Registration  page||Verify that the Password minimum length of 8 characters is ALWAYS enforced in Registration  page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in Registration  page||Verify that error message "Password is too long" whenever enter more than 95 characters||Verify that "View password rules on the right" error message at the time of entering password||Verify that "Should not have leading and trailing spaces" error message at the time of entering password</t>
+  </si>
+  <si>
+    <t>OPQA-5770</t>
+  </si>
+  <si>
+    <t>Verify that error message "Please enter a password." whenever not enter any text in email field</t>
+  </si>
+  <si>
+    <t>PUBLONS014</t>
   </si>
 </sst>
 </file>
@@ -742,14 +760,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="138.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -922,18 +940,34 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added TestCases in Publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -392,6 +392,21 @@
   </si>
   <si>
     <t>PUBLONS017</t>
+  </si>
+  <si>
+    <t>Verify that user account for email address was not found, then auth iframe shows registration page with fn, ln, email prepopulated</t>
+  </si>
+  <si>
+    <t>OPQA-5862</t>
+  </si>
+  <si>
+    <t>PUBLONS019</t>
+  </si>
+  <si>
+    <t>OPQA-5784&amp;&amp;OPQA-5785&amp;&amp;OPQA-5861</t>
+  </si>
+  <si>
+    <t>Verify that "Your email address is already registered. Please sign in." error message whenever try to create publons user using existing account.&amp;&amp;Verify that email address prepopulated in sign in page whenever try to register user using existing user&amp;&amp;Verify that user account for email address was found, then auth iframe shows sign-in page</t>
   </si>
 </sst>
 </file>
@@ -848,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,15 +1028,15 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
@@ -1224,10 +1239,18 @@
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Publons test cases for linking scenario.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="124">
   <si>
     <t>TCID</t>
   </si>
@@ -446,6 +446,24 @@
 Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||
 Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||
 Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page."</t>
+  </si>
+  <si>
+    <t>PUBLONS025</t>
+  </si>
+  <si>
+    <t>OPQA-5893||OPQA-5894||OPQA-5899</t>
+  </si>
+  <si>
+    <t>Verify the linking model should display when user sign in using facebook and enters matching account from the login page||Verify the User is redirected to Publon's Homepage when User enters correct credentials for matching facebook account and Also verify user can see two connected  account on account setting page one is facebook and another is Steam account.||Verify User should not challenged linking model when Facebook is already linked with STeAM.</t>
+  </si>
+  <si>
+    <t>PUBLONS026</t>
+  </si>
+  <si>
+    <t>OPQA-5897||OPQA-5898||OPQA-5999</t>
+  </si>
+  <si>
+    <t>Verify the linking model should display when user sign in using Gmail and enters matching account from the login page||Verify the User is redirected to Publon's Homepage when User enters correct credentials for matching Gmail account and Also verify user can see two connected  account on account setting page one is Gmail and another is Steam account.||Verify User should not challenged linking model when Gmail is already linked with STeAM.</t>
   </si>
 </sst>
 </file>
@@ -902,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,14 +1325,34 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="6"/>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added testcases for publons
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>Verify the linking model should display when user sign in using Gmail and enters matching account from the login page||Verify the User is redirected to Publon's Homepage when User enters correct credentials for matching Gmail account and Also verify user can see two connected  account on account setting page one is Gmail and another is Steam account.||Verify User should not challenged linking model when Gmail is already linked with STeAM.</t>
+  </si>
+  <si>
+    <t>PUBLONS031</t>
+  </si>
+  <si>
+    <t>NILL</t>
+  </si>
+  <si>
+    <t>Add email alias</t>
   </si>
 </sst>
 </file>
@@ -914,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,10 +1365,18 @@
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed Scripts in Publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="122">
   <si>
     <t>TCID</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>OPQA-TBD</t>
-  </si>
-  <si>
-    <t>Verify that user is able to login WoS Author Transformation Application using valid WAT Entitled account</t>
-  </si>
-  <si>
     <t>errorMessage</t>
   </si>
   <si>
@@ -177,16 +171,7 @@
     <t>Verify Error message when user  exist in platform in Evicted state and trying to login.</t>
   </si>
   <si>
-    <t>PUBLONS002</t>
-  </si>
-  <si>
     <t>PUBLONS003</t>
-  </si>
-  <si>
-    <t>OPQA-5765</t>
-  </si>
-  <si>
-    <t>Verify that email address field should be in standard email ID format .Email address fields should be mandatory.</t>
   </si>
   <si>
     <t>Verify that error message "Please enter an email address" whenever not enter any text in email field</t>
@@ -467,6 +452,12 @@
   </si>
   <si>
     <t>Add email alias</t>
+  </si>
+  <si>
+    <t>OPQA-5791</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sign in publons application with STeAM credentials</t>
   </si>
 </sst>
 </file>
@@ -921,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,13 +946,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -970,13 +961,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
@@ -988,55 +979,55 @@
         <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>5</v>
@@ -1045,110 +1036,110 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="D11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="B13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>94</v>
       </c>
@@ -1163,60 +1154,60 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="D16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="345" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="345" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>5</v>
@@ -1225,13 +1216,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>5</v>
@@ -1240,13 +1231,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>5</v>
@@ -1255,13 +1246,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>40</v>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>5</v>
@@ -1270,13 +1261,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>5</v>
@@ -1285,62 +1276,54 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D26" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>5</v>
-      </c>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,25 +1341,25 @@
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,13 +1368,6 @@
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
       <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1411,16 +1387,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,13 +1404,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1442,13 +1418,13 @@
         <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,13 +1432,13 @@
         <v>51</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1482,16 +1458,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,13 +1475,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,13 +1489,13 @@
         <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,13 +1503,13 @@
         <v>51</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1559,22 +1535,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1582,17 +1558,17 @@
         <v>246</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1600,17 +1576,17 @@
         <v>247</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1618,19 +1594,19 @@
         <v>248</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1661,10 +1637,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1675,10 +1651,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1687,10 +1663,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1699,10 +1675,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1711,10 +1687,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1723,10 +1699,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1735,10 +1711,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1747,10 +1723,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1759,10 +1735,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1771,10 +1747,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -1783,10 +1759,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -1795,10 +1771,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -1807,10 +1783,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -1819,10 +1795,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1831,10 +1807,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -1843,10 +1819,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -1855,10 +1831,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1867,10 +1843,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -1879,10 +1855,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
@@ -1891,10 +1867,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
@@ -1903,10 +1879,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
@@ -1915,10 +1891,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
@@ -1927,10 +1903,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1939,10 +1915,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -1951,10 +1927,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -1963,10 +1939,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -1997,10 +1973,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -2011,10 +1987,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2023,10 +1999,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2035,10 +2011,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -2047,10 +2023,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2059,10 +2035,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2071,10 +2047,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -2083,10 +2059,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2095,10 +2071,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -2107,10 +2083,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2119,10 +2095,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -2131,10 +2107,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2143,10 +2119,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -2155,10 +2131,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -2167,10 +2143,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -2179,10 +2155,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -2191,10 +2167,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -2203,10 +2179,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
@@ -2215,10 +2191,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
@@ -2227,10 +2203,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
@@ -2239,10 +2215,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
@@ -2251,10 +2227,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
@@ -2263,10 +2239,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -2275,10 +2251,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -2287,10 +2263,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>5</v>
@@ -2299,10 +2275,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added Linkedln and Steam Linking Scenario Test cases.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>Verify that user is able to sign in publons application with STeAM credentials</t>
+  </si>
+  <si>
+    <t>PUBLONS027</t>
+  </si>
+  <si>
+    <t>OPQA-5895||OPQA-5896||OPQA-5999</t>
+  </si>
+  <si>
+    <t>Verify the linking model should display when user sign in using Linkedln and enters matching account from the login page||Verify the User is redirected to Publon's Homepage when User enters correct credentials for matching Linkedln account and Also verify user can see two connected  account on account setting page one is Linkedln and another is Steam account.||Verify User should not challenged linking model when Linkedln is already linked with STeAM.</t>
   </si>
 </sst>
 </file>
@@ -914,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,11 +1328,19 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="6"/>
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Test cases in xls sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="140">
   <si>
     <t>TCID</t>
   </si>
@@ -467,6 +467,51 @@
   </si>
   <si>
     <t>Verify the linking model should display when user sign in using Linkedln and enters matching account from the login page||Verify the User is redirected to Publon's Homepage when User enters correct credentials for matching Linkedln account and Also verify user can see two connected  account on account setting page one is Linkedln and another is Steam account.||Verify User should not challenged linking model when Linkedln is already linked with STeAM.</t>
+  </si>
+  <si>
+    <t>OPQA-5900</t>
+  </si>
+  <si>
+    <t>Verify user cannot log in and it should display "contact customer support." message when the matching account is already linked to the provider of the signed in user.</t>
+  </si>
+  <si>
+    <t>PUBLONS028</t>
+  </si>
+  <si>
+    <t>OPQA-5901</t>
+  </si>
+  <si>
+    <t>OPQA-5902</t>
+  </si>
+  <si>
+    <t>PUBLONS029</t>
+  </si>
+  <si>
+    <t>PUBLONS030</t>
+  </si>
+  <si>
+    <t>PUBLONS032</t>
+  </si>
+  <si>
+    <t>OPQA-5903</t>
+  </si>
+  <si>
+    <t>OPQA-5904</t>
+  </si>
+  <si>
+    <t>PUBLONS033</t>
+  </si>
+  <si>
+    <t>Verify user cannot log in and it should display appropriate error messag when Matching account exist in platform but in blocked state.</t>
+  </si>
+  <si>
+    <t>Verify user cannot log in and it should display appropriate error message when Matching account exist in platform but in evicted state.</t>
+  </si>
+  <si>
+    <t>Verify user cannot log in and it should display appropriate error message when Matching account exist in platform but in locked state.</t>
+  </si>
+  <si>
+    <t>Verify user cannot log in and it should display appropriate error message when Matching account  registered but not activated.</t>
   </si>
 </sst>
 </file>
@@ -921,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,52 +1388,93 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="D32" s="6"/>
       <c r="E32" s="8"/>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="8"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B29:B30" r:id="rId1" display="https://jira.clarivate.io/browse/OPQA-5898"/>
+    <hyperlink ref="B32:B33" r:id="rId2" display="https://jira.clarivate.io/browse/OPQA-5898"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Test scripts PUBLONS028.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="140">
   <si>
     <t>TCID</t>
   </si>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,7 +1398,9 @@
       <c r="C28" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,7 +1413,9 @@
       <c r="C29" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,7 +1428,9 @@
       <c r="C30" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1452,7 +1458,9 @@
       <c r="C32" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,7 +1473,9 @@
       <c r="C33" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E33" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Publons xls sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="148">
   <si>
     <t>TCID</t>
   </si>
@@ -512,6 +512,30 @@
   </si>
   <si>
     <t>Verify User able to add alias account after click on "Add email address" and enter valid emil id .</t>
+  </si>
+  <si>
+    <t>PUBLONS034</t>
+  </si>
+  <si>
+    <t>PUBLONS035</t>
+  </si>
+  <si>
+    <t>PUBLONS036</t>
+  </si>
+  <si>
+    <t>PUBLONS037</t>
+  </si>
+  <si>
+    <t>PUBLONS038</t>
+  </si>
+  <si>
+    <t>PUBLONS039</t>
+  </si>
+  <si>
+    <t>PUBLONS040</t>
+  </si>
+  <si>
+    <t>PUBLONS041</t>
   </si>
 </sst>
 </file>
@@ -612,7 +636,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -633,6 +657,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -966,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,36 +1479,143 @@
       <c r="A32" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="8"/>
+      <c r="D41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B29:B30" r:id="rId1" display="https://jira.clarivate.io/browse/OPQA-5898"/>
-    <hyperlink ref="B32:B33" r:id="rId2" display="https://jira.clarivate.io/browse/OPQA-5898"/>
+    <hyperlink ref="B40:B41" r:id="rId2" display="https://jira.clarivate.io/browse/OPQA-5898"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Added Publons Test scripts 030.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="147">
   <si>
     <t>TCID</t>
   </si>
@@ -470,9 +470,6 @@
   </si>
   <si>
     <t>PUBLONS028</t>
-  </si>
-  <si>
-    <t>OPQA-5901</t>
   </si>
   <si>
     <t>OPQA-5902</t>
@@ -995,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,13 +1429,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>126</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>5</v>
@@ -1447,13 +1444,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>5</v>
@@ -1465,10 +1462,10 @@
         <v>117</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>5</v>
@@ -1477,7 +1474,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="12"/>
@@ -1486,7 +1483,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="2"/>
       <c r="D33" s="2"/>
@@ -1494,7 +1491,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="12"/>
@@ -1503,7 +1500,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="12"/>
@@ -1512,7 +1509,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="12"/>
@@ -1521,7 +1518,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="12"/>
@@ -1530,7 +1527,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="12"/>
@@ -1539,7 +1536,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="12"/>
@@ -1548,13 +1545,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>5</v>
@@ -1563,13 +1560,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>5</v>
@@ -1613,11 +1610,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29:B30" r:id="rId1" display="https://jira.clarivate.io/browse/OPQA-5898"/>
-    <hyperlink ref="B40:B41" r:id="rId2" display="https://jira.clarivate.io/browse/OPQA-5898"/>
+    <hyperlink ref="B40:B41" r:id="rId1" display="https://jira.clarivate.io/browse/OPQA-5898"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Test scripts for linking error message.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="153">
   <si>
     <t>TCID</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>Verify error message user didn't enter correct password when matching account exist in STeAM and user sign in using facebook  from login page and enters incorrect password for matching account.</t>
+  </si>
+  <si>
+    <t>Verify error message user didn't enter correct password when matching account exist in STeAM and user sign in using Gmail  from login page and enters incorrect password for matching account.</t>
+  </si>
+  <si>
+    <t>Verify error message user didn't enter correct password when matching account exist in STeAM and user sign in using Linkedln  from login page and enters incorrect password for matching account.</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1602,7 @@
         <v>148</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>5</v>
@@ -1611,7 +1617,7 @@
         <v>149</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Created new test case for publons module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/PUBLONS.xlsx
+++ b/src/test/resources/xls/PUBLONS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -499,12 +499,6 @@
     <t>Verify user cannot log in and it should display appropriate error message when Matching account  registered but not activated.</t>
   </si>
   <si>
-    <t>OPQA-5993</t>
-  </si>
-  <si>
-    <t>Verify User able to add alias account after click on "Add email address" and enter valid emil id .</t>
-  </si>
-  <si>
     <t>PUBLONS034</t>
   </si>
   <si>
@@ -551,6 +545,18 @@
   </si>
   <si>
     <t>Verify error message user didn't enter correct password when matching account exist in STeAM and user sign in using Linkedln  from login page and enters incorrect password for matching account.</t>
+  </si>
+  <si>
+    <t>OPQA-5993||OPQA-5995</t>
+  </si>
+  <si>
+    <t>Verify User able to add alias account after click on "Add email address" and  Verify that user received activation link,after click on activation link user is created and navigating to account setting page</t>
+  </si>
+  <si>
+    <t>Verify user can switch primary account within added alias account</t>
+  </si>
+  <si>
+    <t>OPQA-5998</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1020,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,15 +1484,15 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>5</v>
@@ -1497,9 +1503,15 @@
       <c r="A32" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,7 +1524,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="12"/>
@@ -1521,7 +1533,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="12"/>
@@ -1530,7 +1542,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="12"/>
@@ -1539,7 +1551,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="12"/>
@@ -1548,7 +1560,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="12"/>
@@ -1557,7 +1569,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="12"/>
@@ -1566,7 +1578,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>130</v>
@@ -1581,13 +1593,13 @@
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>5</v>
@@ -1596,13 +1608,13 @@
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>5</v>
@@ -1611,13 +1623,13 @@
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>5</v>

</xml_diff>